<commit_message>
feat: signing and coockies
</commit_message>
<xml_diff>
--- a/stepByStepTesting.xlsx
+++ b/stepByStepTesting.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">This is based on p106 of "ISO/IEC/IEEE International Standard - Software and systems engineering -- Software testing --Part 3: Test documentation," in ISO/IEC/IEEE 29119-3:2013(E) , vol., no., pp.1-138, 1 Sept. 2013, doi: 10.1109/IEEESTD.2013.6588540.
 https://ieeexplore.ieee.org/document/6588540
@@ -32,13 +32,13 @@
 Duration:</t>
   </si>
   <si>
-    <t xml:space="preserve">To test the behaviour of the password entry box under various conditions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Startup: Open browser, go to domain.com/login page</t>
+    <t xml:space="preserve">User must be able to create a new account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Startup: Start server, open browser, go to localhost:5000/login page</t>
   </si>
   <si>
     <t xml:space="preserve">Relationship to other procedures: none</t>
@@ -59,6 +59,15 @@
     <t xml:space="preserve">Ok/ not ok</t>
   </si>
   <si>
+    <t>31/08/2021</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comments: </t>
   </si>
   <si>
@@ -80,36 +89,18 @@
     <t xml:space="preserve">Test result</t>
   </si>
   <si>
-    <t xml:space="preserve">Type in ‘test’ to the password box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check that four stars appear in the password box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Four stars appeared</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop and wrap up. Clear browser data and close window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User must be able to create a new account</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Startup: Start server, open browser, go to localhost:5000/login page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Type in 'bob' into username, 'bob1' into password, 'bob2' into password 2</t>
   </si>
   <si>
     <t xml:space="preserve">Check for error message below submit button should say 'passwords do not match'</t>
   </si>
   <si>
+    <t xml:space="preserve">message matched</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type in 'bob' into all text boxes</t>
   </si>
   <si>
@@ -120,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">Leave all text boxes blank and submit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check response message should say 'All fields must be filled'</t>
   </si>
   <si>
     <t xml:space="preserve">Stop and wrap up. delete the user from database.</t>
@@ -228,17 +222,16 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
@@ -258,6 +251,9 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -711,387 +707,267 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="3" ht="38.25">
-      <c r="B3" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="3" ht="12.75">
+      <c r="D3"/>
+    </row>
+    <row r="4" ht="12.75">
+      <c r="D4"/>
+    </row>
+    <row r="5" ht="38.25">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="24.050000000000001">
-      <c r="B4" s="4">
-        <v>123</v>
-      </c>
-      <c r="C4" s="5" t="s">
+    <row r="6" ht="12.75">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="29.199999999999999" customHeight="1">
-      <c r="B5" s="4" t="s">
+    <row r="7" ht="12.75">
+      <c r="B7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" ht="12.800000000000001">
-      <c r="B6" s="4" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" ht="12.75">
+      <c r="B8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" ht="12.800000000000001">
-      <c r="B7" s="3" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" ht="12.800000000000001">
-      <c r="B8" s="2" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" ht="12.75">
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" ht="12.800000000000001">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" ht="12.800000000000001">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" ht="12.800000000000001">
-      <c r="B11" s="4" t="s">
+    <row r="11" ht="12.75">
+      <c r="B11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" ht="12.800000000000001">
-      <c r="B12" s="3" t="s">
+      <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" ht="25.5">
-      <c r="B13" s="2" t="s">
+      <c r="D11" s="11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+    </row>
+    <row r="12" ht="12.75">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" ht="12.75">
+      <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" ht="25.5">
+      <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" ht="51">
-      <c r="B14" s="4">
+      <c r="D15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" ht="89.25">
+      <c r="B16" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="C16" s="16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" ht="12.800000000000001">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" ht="12.800000000000001">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" ht="12.800000000000001">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" ht="12.800000000000001">
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" ht="12.800000000000001">
-      <c r="B19" s="4" t="s">
+      <c r="D16" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="22" ht="38.25">
-      <c r="B22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" ht="12.75">
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="E16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" ht="12.75">
-      <c r="B24" s="13" t="s">
+    <row r="17" ht="38.25">
+      <c r="B17" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-    </row>
-    <row r="25" ht="12.75">
-      <c r="B25" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-    </row>
-    <row r="26" ht="12.75">
-      <c r="B26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
-    </row>
+      <c r="D17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" ht="38.25">
+      <c r="B18" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" ht="51">
+      <c r="B19" s="7">
+        <v>1.3999999999999999</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" ht="12.75">
+      <c r="B20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="22" ht="12.75"/>
+    <row r="23" ht="12.75"/>
+    <row r="24" ht="12.75"/>
+    <row r="25" ht="12.75"/>
+    <row r="26" ht="12.75"/>
     <row r="27" ht="12.75">
-      <c r="B27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="8"/>
-      <c r="F27" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="D27"/>
     </row>
     <row r="28" ht="12.75">
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="D28"/>
     </row>
     <row r="29" ht="12.75">
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" ht="12.75">
-      <c r="B30" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="15"/>
-    </row>
-    <row r="31" ht="12.75">
-      <c r="B31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" ht="25.5">
-      <c r="B32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" ht="89.25">
-      <c r="B33" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" ht="38.25">
-      <c r="B34" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" ht="38.25">
-      <c r="B35" s="4">
-        <v>1.3</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" ht="51">
-      <c r="B36" s="4">
-        <v>1.3999999999999999</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="D29"/>
+    </row>
+    <row r="30" ht="12.75"/>
+    <row r="31" ht="12.75"/>
+    <row r="32" ht="12.75">
+      <c r="D32"/>
+    </row>
+    <row r="33" ht="12.75">
+      <c r="D33"/>
+    </row>
+    <row r="34" ht="12.75">
+      <c r="D34"/>
+    </row>
+    <row r="35" ht="12.75">
+      <c r="D35"/>
+    </row>
+    <row r="36" ht="12.75">
+      <c r="D36"/>
     </row>
     <row r="37" ht="12.75">
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-    </row>
-    <row r="38" ht="12.75">
-      <c r="B38" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
-    </row>
+      <c r="D37"/>
+    </row>
+    <row r="38" ht="12.75"/>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="10">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.05277777777778" bottom="1.05277777777778" header="0.78750000000000009" footer="0.78750000000000009"/>

</xml_diff>

<commit_message>
test: user sign in
</commit_message>
<xml_diff>
--- a/stepByStepTesting.xlsx
+++ b/stepByStepTesting.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">This is based on p106 of "ISO/IEC/IEEE International Standard - Software and systems engineering -- Software testing --Part 3: Test documentation," in ISO/IEC/IEEE 29119-3:2013(E) , vol., no., pp.1-138, 1 Sept. 2013, doi: 10.1109/IEEESTD.2013.6588540.
 https://ieeexplore.ieee.org/document/6588540
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>902/9/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Comments: </t>
@@ -217,11 +220,8 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
@@ -241,11 +241,10 @@
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
@@ -254,9 +253,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -707,254 +703,240 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="3" ht="12.75">
-      <c r="D3"/>
-    </row>
-    <row r="4" ht="12.75">
-      <c r="D4"/>
-    </row>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="3" ht="12.75"/>
+    <row r="4" ht="12.75"/>
     <row r="5" ht="38.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="12.75">
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="12.75">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" ht="12.75">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" ht="12.75">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" ht="12.75">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" ht="12.75">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="6">
         <v>1</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" ht="12.75">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" ht="12.75">
-      <c r="B13" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
+      <c r="B13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" ht="12.75">
-      <c r="B14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" ht="25.5">
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F15" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" ht="89.25">
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="D16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="14" t="s">
         <v>26</v>
       </c>
+      <c r="F16" s="6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="17" ht="38.25">
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>1.2</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="17" t="s">
+    </row>
+    <row r="18" ht="38.25">
+      <c r="B18" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="11" t="s">
+      <c r="D18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" ht="38.25">
-      <c r="B18" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="C18" s="19" t="s">
+      <c r="F18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="11" t="s">
+    </row>
+    <row r="19" ht="51">
+      <c r="B19" s="6">
+        <v>1.3999999999999999</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" ht="51">
-      <c r="B19" s="7">
-        <v>1.3999999999999999</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>26</v>
+      <c r="F19" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" ht="12.75">
-      <c r="B20" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
+      <c r="B20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="22" ht="12.75"/>
     <row r="23" ht="12.75"/>
     <row r="24" ht="12.75"/>
     <row r="25" ht="12.75"/>
     <row r="26" ht="12.75"/>
-    <row r="27" ht="12.75">
-      <c r="D27"/>
-    </row>
-    <row r="28" ht="12.75">
-      <c r="D28"/>
-    </row>
-    <row r="29" ht="12.75">
-      <c r="D29"/>
-    </row>
+    <row r="27" ht="12.75"/>
+    <row r="28" ht="12.75"/>
+    <row r="29" ht="12.75"/>
     <row r="30" ht="12.75"/>
     <row r="31" ht="12.75"/>
-    <row r="32" ht="12.75">
-      <c r="D32"/>
-    </row>
-    <row r="33" ht="12.75">
-      <c r="D33"/>
-    </row>
-    <row r="34" ht="12.75">
-      <c r="D34"/>
-    </row>
-    <row r="35" ht="12.75">
-      <c r="D35"/>
-    </row>
-    <row r="36" ht="12.75">
-      <c r="D36"/>
-    </row>
-    <row r="37" ht="12.75">
-      <c r="D37"/>
-    </row>
+    <row r="32" ht="12.75"/>
+    <row r="33" ht="12.75"/>
+    <row r="34" ht="12.75"/>
+    <row r="35" ht="12.75"/>
+    <row r="36" ht="12.75"/>
+    <row r="37" ht="12.75"/>
     <row r="38" ht="12.75"/>
   </sheetData>
   <mergeCells count="10">

</xml_diff>